<commit_message>
Finish Service,Testimonial by Tham Vinh Thanh
</commit_message>
<xml_diff>
--- a/template_task.xlsx
+++ b/template_task.xlsx
@@ -1,30 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarcusCheung\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d7b22d395baaf5d7/Máy tính/cyber_capstone_tailwind/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_818B203B6DAC5C7714F5192EDA33B6FF8EC4C10A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9BE091D-7C4D-4EA4-8A25-B3E32E2794FE}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -159,7 +173,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd"/>
   </numFmts>
@@ -340,8 +354,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="21">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -372,10 +386,7 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="3" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -385,13 +396,7 @@
     <xf numFmtId="9" fontId="3" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="9" fontId="3" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -411,29 +416,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -666,14 +649,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:J985"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
@@ -725,10 +708,10 @@
       <c r="A2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="11">
+      <c r="B2" s="8">
         <v>45586</v>
       </c>
-      <c r="C2" s="11">
+      <c r="C2" s="8">
         <v>45586</v>
       </c>
       <c r="D2" s="9">
@@ -737,127 +720,127 @@
       <c r="E2" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="11"/>
+      <c r="F2" s="8"/>
       <c r="G2" s="8"/>
-      <c r="H2" s="12"/>
+      <c r="H2" s="11"/>
       <c r="I2" s="10"/>
-      <c r="J2" s="13"/>
+      <c r="J2" s="12"/>
     </row>
     <row r="3" spans="1:10" ht="14.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="15">
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="14">
         <v>0.5</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="11"/>
+      <c r="F3" s="8"/>
       <c r="G3" s="8"/>
-      <c r="H3" s="17"/>
+      <c r="H3" s="15"/>
       <c r="I3" s="10"/>
-      <c r="J3" s="13"/>
+      <c r="J3" s="12"/>
     </row>
     <row r="4" spans="1:10" ht="14.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4" s="8">
         <v>43608</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="8">
         <v>43647</v>
       </c>
-      <c r="D4" s="19">
+      <c r="D4" s="16">
         <f>SUM(D5:D7)/3</f>
         <v>0.9</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="11"/>
+      <c r="F4" s="8"/>
       <c r="G4" s="8"/>
-      <c r="H4" s="20"/>
+      <c r="H4" s="17"/>
       <c r="I4" s="10"/>
-      <c r="J4" s="13"/>
+      <c r="J4" s="12"/>
     </row>
     <row r="5" spans="1:10" ht="14.25" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="21">
+      <c r="B5" s="18">
         <v>43608</v>
       </c>
-      <c r="C5" s="21">
+      <c r="C5" s="18">
         <v>43616</v>
       </c>
-      <c r="D5" s="19">
+      <c r="D5" s="16">
         <v>1</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="21"/>
+      <c r="F5" s="18"/>
       <c r="G5" s="8"/>
-      <c r="H5" s="20"/>
+      <c r="H5" s="17"/>
       <c r="I5" s="10"/>
-      <c r="J5" s="13"/>
+      <c r="J5" s="12"/>
     </row>
     <row r="6" spans="1:10" ht="14.25" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="21">
+      <c r="B6" s="18">
         <v>43636</v>
       </c>
-      <c r="C6" s="21">
+      <c r="C6" s="18">
         <v>43644</v>
       </c>
-      <c r="D6" s="19">
+      <c r="D6" s="16">
         <v>0.9</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="E6" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="21"/>
+      <c r="F6" s="18"/>
       <c r="G6" s="8"/>
-      <c r="H6" s="20"/>
+      <c r="H6" s="17"/>
       <c r="I6" s="10"/>
-      <c r="J6" s="13"/>
+      <c r="J6" s="12"/>
     </row>
     <row r="7" spans="1:10" ht="14.25" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="21">
+      <c r="B7" s="18">
         <v>43641</v>
       </c>
-      <c r="C7" s="21">
+      <c r="C7" s="18">
         <v>43647</v>
       </c>
-      <c r="D7" s="19">
+      <c r="D7" s="16">
         <v>0.8</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="21"/>
+      <c r="F7" s="18"/>
       <c r="G7" s="8"/>
-      <c r="H7" s="20"/>
+      <c r="H7" s="17"/>
       <c r="I7" s="10"/>
-      <c r="J7" s="22"/>
+      <c r="J7" s="19"/>
     </row>
     <row r="8" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="11">
+      <c r="B8" s="8">
         <v>45585</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="8">
         <v>45585</v>
       </c>
       <c r="D8" s="9">
@@ -866,257 +849,275 @@
       <c r="E8" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="11"/>
+      <c r="F8" s="8"/>
       <c r="G8" s="8"/>
-      <c r="H8" s="12"/>
+      <c r="H8" s="11"/>
       <c r="I8" s="10"/>
-      <c r="J8" s="13"/>
+      <c r="J8" s="12"/>
     </row>
     <row r="9" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="11">
+      <c r="B9" s="8">
         <v>45586</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="8">
         <v>45586</v>
       </c>
       <c r="D9" s="9">
         <v>1</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="E9" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="11"/>
+      <c r="F9" s="8"/>
       <c r="G9" s="8"/>
-      <c r="H9" s="12"/>
+      <c r="H9" s="11"/>
       <c r="I9" s="10"/>
-      <c r="J9" s="13"/>
+      <c r="J9" s="12"/>
     </row>
     <row r="10" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="11">
+      <c r="B10" s="8">
         <v>45585</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C10" s="8">
         <v>45585</v>
       </c>
       <c r="D10" s="9">
         <v>1</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="E10" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="11"/>
+      <c r="F10" s="8"/>
       <c r="G10" s="8"/>
-      <c r="H10" s="12"/>
+      <c r="H10" s="11"/>
       <c r="I10" s="10"/>
-      <c r="J10" s="13"/>
+      <c r="J10" s="12"/>
     </row>
     <row r="11" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="11">
+      <c r="B11" s="8">
         <v>45588</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="8">
         <v>45588</v>
       </c>
       <c r="D11" s="9">
         <v>1</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="F11" s="11"/>
+      <c r="F11" s="8"/>
       <c r="G11" s="8"/>
-      <c r="H11" s="12"/>
+      <c r="H11" s="11"/>
       <c r="I11" s="10"/>
-      <c r="J11" s="13"/>
+      <c r="J11" s="12"/>
     </row>
     <row r="12" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="11">
+      <c r="B12" s="8">
         <v>45586</v>
       </c>
-      <c r="C12" s="11">
+      <c r="C12" s="8">
         <v>45586</v>
       </c>
       <c r="D12" s="9">
         <v>1</v>
       </c>
-      <c r="E12" s="16" t="s">
+      <c r="E12" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="F12" s="11"/>
+      <c r="F12" s="8"/>
       <c r="G12" s="8"/>
-      <c r="H12" s="12"/>
+      <c r="H12" s="11"/>
       <c r="I12" s="10"/>
-      <c r="J12" s="13"/>
+      <c r="J12" s="12"/>
     </row>
     <row r="13" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="23" t="s">
+      <c r="A13" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="16" t="s">
+      <c r="B13" s="8">
+        <v>45588</v>
+      </c>
+      <c r="C13" s="8">
+        <v>45588</v>
+      </c>
+      <c r="D13" s="9">
+        <v>1</v>
+      </c>
+      <c r="E13" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="F13" s="11"/>
+      <c r="F13" s="8"/>
       <c r="G13" s="8"/>
-      <c r="H13" s="12"/>
+      <c r="H13" s="11"/>
       <c r="I13" s="10"/>
-      <c r="J13" s="13"/>
+      <c r="J13" s="12"/>
     </row>
     <row r="14" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="11">
+      <c r="B14" s="8">
         <v>45587</v>
       </c>
-      <c r="C14" s="11">
+      <c r="C14" s="8">
         <v>45587</v>
       </c>
       <c r="D14" s="9">
         <v>1</v>
       </c>
-      <c r="E14" s="16" t="s">
+      <c r="E14" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="F14" s="11"/>
+      <c r="F14" s="8"/>
       <c r="G14" s="8"/>
-      <c r="H14" s="12"/>
+      <c r="H14" s="11"/>
       <c r="I14" s="10"/>
-      <c r="J14" s="13"/>
+      <c r="J14" s="12"/>
     </row>
     <row r="15" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="11">
+      <c r="B15" s="8">
         <v>45588</v>
       </c>
-      <c r="C15" s="11">
+      <c r="C15" s="8">
         <v>45588</v>
       </c>
       <c r="D15" s="9">
         <v>1</v>
       </c>
-      <c r="E15" s="16" t="s">
+      <c r="E15" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="13"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="12"/>
     </row>
     <row r="16" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="23" t="s">
+      <c r="A16" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="11">
+      <c r="B16" s="8">
         <v>45588</v>
       </c>
-      <c r="C16" s="11">
+      <c r="C16" s="8">
         <v>45588</v>
       </c>
       <c r="D16" s="9">
         <v>1</v>
       </c>
-      <c r="E16" s="16" t="s">
+      <c r="E16" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="13"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="12"/>
     </row>
     <row r="17" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="23" t="s">
+      <c r="A17" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="16" t="s">
+      <c r="B17" s="8">
+        <v>45589</v>
+      </c>
+      <c r="C17" s="8">
+        <v>45589</v>
+      </c>
+      <c r="D17" s="9">
+        <v>1</v>
+      </c>
+      <c r="E17" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="13"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="12"/>
     </row>
     <row r="18" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="23" t="s">
+      <c r="A18" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="11">
+      <c r="B18" s="8">
         <v>45588</v>
       </c>
-      <c r="C18" s="11">
+      <c r="C18" s="8">
         <v>45588</v>
       </c>
       <c r="D18" s="9">
         <v>1</v>
       </c>
-      <c r="E18" s="16" t="s">
+      <c r="E18" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="13"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="12"/>
     </row>
     <row r="19" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="23" t="s">
+      <c r="A19" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="16" t="s">
+      <c r="B19" s="8">
+        <v>45589</v>
+      </c>
+      <c r="C19" s="8">
+        <v>45589</v>
+      </c>
+      <c r="D19" s="9">
+        <v>1</v>
+      </c>
+      <c r="E19" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="16"/>
-      <c r="J19" s="13"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="12"/>
     </row>
     <row r="20" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="23" t="s">
+      <c r="A20" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="11">
+      <c r="B20" s="8">
         <v>45588</v>
       </c>
-      <c r="C20" s="11">
+      <c r="C20" s="8">
         <v>45588</v>
       </c>
       <c r="D20" s="9">
         <v>1</v>
       </c>
-      <c r="E20" s="16" t="s">
+      <c r="E20" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="16"/>
-      <c r="J20" s="13"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="12"/>
     </row>
     <row r="21" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2085,12 +2086,12 @@
     <row r="985" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="D2 D4:D20">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2 H4:H20">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Fix by Tham Vinh Thanh
</commit_message>
<xml_diff>
--- a/template_task.xlsx
+++ b/template_task.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d7b22d395baaf5d7/Máy tính/cyber_capstone_tailwind/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_818B203B6DAC5C7714F5192EDA33B6FF8EC4C10A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9BE091D-7C4D-4EA4-8A25-B3E32E2794FE}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_818B203B6DAC5C7714F5192EDA33B6FF8EC4C10A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7561568B-2697-4B24-8361-4FAFFB8F7D3E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,8 +24,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -69,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="32">
   <si>
     <t>Tasks Name</t>
   </si>
@@ -168,6 +166,9 @@
   </si>
   <si>
     <t>Footer</t>
+  </si>
+  <si>
+    <t>Sử dụng thư viện Slick thay cho thư viện Swiper</t>
   </si>
 </sst>
 </file>
@@ -656,7 +657,7 @@
   <dimension ref="A1:J985"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
@@ -963,7 +964,9 @@
       <c r="G13" s="8"/>
       <c r="H13" s="11"/>
       <c r="I13" s="10"/>
-      <c r="J13" s="12"/>
+      <c r="J13" s="12" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="14" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
@@ -1051,7 +1054,9 @@
       <c r="G17" s="8"/>
       <c r="H17" s="11"/>
       <c r="I17" s="10"/>
-      <c r="J17" s="12"/>
+      <c r="J17" s="12" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="18" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">

</xml_diff>